<commit_message>
update with new data
</commit_message>
<xml_diff>
--- a/data/season_start_stop.xlsx
+++ b/data/season_start_stop.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\GwentRankGit\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40F50456-2112-4F4C-AC00-AA8B0E7FDDFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78A18FEB-EF03-4139-9BD1-792E29237946}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12690" yWindow="2910" windowWidth="20145" windowHeight="12600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="87">
   <si>
     <t>season</t>
   </si>
@@ -244,6 +244,48 @@
   </si>
   <si>
     <t>Start Tissaia Journey</t>
+  </si>
+  <si>
+    <t>9.3</t>
+  </si>
+  <si>
+    <t>M3_09 Dryad 2021</t>
+  </si>
+  <si>
+    <t>Only balance changes/bug fixes</t>
+  </si>
+  <si>
+    <t>M3_10 Cat 2021</t>
+  </si>
+  <si>
+    <t>M3_11 Mahakam 2021</t>
+  </si>
+  <si>
+    <t>M3_12 Wild Hunt 2021</t>
+  </si>
+  <si>
+    <t>M4_01 Wolf 2022</t>
+  </si>
+  <si>
+    <t>9.4</t>
+  </si>
+  <si>
+    <t>New Expansion! Harvest of Sorrow</t>
+  </si>
+  <si>
+    <t>9.5</t>
+  </si>
+  <si>
+    <t>Start Regis Journey</t>
+  </si>
+  <si>
+    <t>9.6</t>
+  </si>
+  <si>
+    <t>10.1</t>
+  </si>
+  <si>
+    <t>Draft out of early access</t>
   </si>
 </sst>
 </file>
@@ -577,22 +619,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.5546875" customWidth="1"/>
-    <col min="5" max="5" width="36.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="63.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" customWidth="1"/>
+    <col min="5" max="5" width="36.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="63.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -612,7 +654,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -632,7 +674,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -649,7 +691,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -669,7 +711,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -689,7 +731,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -706,7 +748,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -723,7 +765,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -740,7 +782,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -757,7 +799,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -777,7 +819,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -797,7 +839,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -814,7 +856,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -831,7 +873,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -851,7 +893,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>51</v>
       </c>
@@ -871,7 +913,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>56</v>
       </c>
@@ -891,7 +933,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>59</v>
       </c>
@@ -909,7 +951,7 @@
       </c>
       <c r="F17" s="1"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>61</v>
       </c>
@@ -926,7 +968,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>62</v>
       </c>
@@ -943,7 +985,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>65</v>
       </c>
@@ -963,13 +1005,16 @@
         <v>29</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>69</v>
       </c>
       <c r="B21" s="1">
         <v>44411</v>
       </c>
+      <c r="C21" s="1">
+        <v>44441</v>
+      </c>
       <c r="D21" s="1" t="s">
         <v>70</v>
       </c>
@@ -978,6 +1023,92 @@
       </c>
       <c r="F21" s="1" t="s">
         <v>72</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>74</v>
+      </c>
+      <c r="B22" s="1">
+        <v>44441</v>
+      </c>
+      <c r="C22" s="1">
+        <v>44474</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E22" t="s">
+        <v>75</v>
+      </c>
+      <c r="F22" s="1"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>76</v>
+      </c>
+      <c r="B23" s="1">
+        <v>44474</v>
+      </c>
+      <c r="C23" s="1">
+        <v>44497</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E23" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>77</v>
+      </c>
+      <c r="B24" s="1">
+        <v>44497</v>
+      </c>
+      <c r="C24" s="1">
+        <v>44537</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E24" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>78</v>
+      </c>
+      <c r="B25" s="1">
+        <v>44537</v>
+      </c>
+      <c r="C25" s="1">
+        <v>44574</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E25" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>79</v>
+      </c>
+      <c r="B26" s="1">
+        <v>44574</v>
+      </c>
+      <c r="C26" s="1">
+        <v>44600</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="E26" t="s">
+        <v>86</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated data, faster version to get popularity
</commit_message>
<xml_diff>
--- a/data/season_start_stop.xlsx
+++ b/data/season_start_stop.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\GwentRankGit\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78A18FEB-EF03-4139-9BD1-792E29237946}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AD3BB69-9F11-42F1-A8A1-743F95280BF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12690" yWindow="2910" windowWidth="20145" windowHeight="12600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7455" yWindow="1560" windowWidth="26835" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="90">
   <si>
     <t>season</t>
   </si>
@@ -286,6 +286,15 @@
   </si>
   <si>
     <t>Draft out of early access</t>
+  </si>
+  <si>
+    <t>10.2</t>
+  </si>
+  <si>
+    <t>Start Dandelion Journey</t>
+  </si>
+  <si>
+    <t>M4_02 Love 2022</t>
   </si>
 </sst>
 </file>
@@ -619,10 +628,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F26"/>
+  <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1111,6 +1120,23 @@
         <v>86</v>
       </c>
     </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>89</v>
+      </c>
+      <c r="B27" s="1">
+        <v>44600</v>
+      </c>
+      <c r="C27" s="1">
+        <v>44628</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E27" t="s">
+        <v>88</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>